<commit_message>
Added stacked bar + cumulative plot
</commit_message>
<xml_diff>
--- a/BAU_Floating_Gantt.xlsx
+++ b/BAU_Floating_Gantt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mshields\Documents\Projects\Supply Chain Roadmap\WETO requests\PTC_ITC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A9E849-C9E4-450D-9308-402D8EE24DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E290E850-F4C8-4F51-B12B-9AA39351A0C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{53585B98-3EE9-4F0B-A243-A3207BC010B9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{53585B98-3EE9-4F0B-A243-A3207BC010B9}"/>
   </bookViews>
   <sheets>
     <sheet name="BAU" sheetId="1" r:id="rId1"/>
@@ -621,8 +621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99FEF727-7431-4502-9BF2-797477A5DFA8}">
   <dimension ref="A1:R22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22:O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -836,6 +836,39 @@
         <f t="shared" ref="D5:E5" si="0">D4/12</f>
         <v>166.66666666666666</v>
       </c>
+      <c r="E5" s="24">
+        <v>0</v>
+      </c>
+      <c r="F5" s="24">
+        <v>0</v>
+      </c>
+      <c r="G5" s="24">
+        <v>0</v>
+      </c>
+      <c r="H5" s="24">
+        <v>0</v>
+      </c>
+      <c r="I5" s="24">
+        <v>0</v>
+      </c>
+      <c r="J5" s="24">
+        <v>0</v>
+      </c>
+      <c r="K5" s="24">
+        <v>0</v>
+      </c>
+      <c r="L5" s="24">
+        <v>0</v>
+      </c>
+      <c r="M5" s="24">
+        <v>0</v>
+      </c>
+      <c r="N5" s="24">
+        <v>0</v>
+      </c>
+      <c r="O5" s="24">
+        <v>0</v>
+      </c>
       <c r="P5" t="s">
         <v>22</v>
       </c>
@@ -847,8 +880,12 @@
       <c r="B6" s="11">
         <v>0</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
+      <c r="C6" s="29">
+        <v>0</v>
+      </c>
+      <c r="D6" s="29">
+        <v>0</v>
+      </c>
       <c r="E6" s="1">
         <f>E4/15</f>
         <v>133.33333333333334</v>
@@ -873,10 +910,21 @@
         <f>J4/15</f>
         <v>133.33333333333334</v>
       </c>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
+      <c r="K6" s="24">
+        <v>0</v>
+      </c>
+      <c r="L6" s="24">
+        <v>0</v>
+      </c>
+      <c r="M6" s="24">
+        <v>0</v>
+      </c>
+      <c r="N6" s="24">
+        <v>0</v>
+      </c>
+      <c r="O6" s="24">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:18" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="9" t="s">
@@ -885,14 +933,30 @@
       <c r="B7" s="12">
         <v>0</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
+      <c r="C7" s="30">
+        <v>0</v>
+      </c>
+      <c r="D7" s="30">
+        <v>0</v>
+      </c>
+      <c r="E7" s="12">
+        <v>0</v>
+      </c>
+      <c r="F7" s="30">
+        <v>0</v>
+      </c>
+      <c r="G7" s="30">
+        <v>0</v>
+      </c>
+      <c r="H7" s="30">
+        <v>0</v>
+      </c>
+      <c r="I7" s="30">
+        <v>0</v>
+      </c>
+      <c r="J7" s="30">
+        <v>0</v>
+      </c>
       <c r="K7" s="1">
         <f>K4/18</f>
         <v>111.11111111111111</v>
@@ -1715,18 +1779,45 @@
       <c r="B22" s="6">
         <v>0</v>
       </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
-      <c r="M22" s="6"/>
-      <c r="N22" s="6"/>
+      <c r="C22" s="24">
+        <v>0</v>
+      </c>
+      <c r="D22" s="24">
+        <v>0</v>
+      </c>
+      <c r="E22" s="24">
+        <v>0</v>
+      </c>
+      <c r="F22" s="24">
+        <v>0</v>
+      </c>
+      <c r="G22" s="24">
+        <v>0</v>
+      </c>
+      <c r="H22" s="24">
+        <v>0</v>
+      </c>
+      <c r="I22" s="24">
+        <v>0</v>
+      </c>
+      <c r="J22" s="24">
+        <v>0</v>
+      </c>
+      <c r="K22" s="24">
+        <v>0</v>
+      </c>
+      <c r="L22" s="24">
+        <v>0</v>
+      </c>
+      <c r="M22" s="24">
+        <v>0</v>
+      </c>
+      <c r="N22" s="24">
+        <v>0</v>
+      </c>
+      <c r="O22" s="24">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1737,8 +1828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FBFDA7F-5F64-4EB0-B210-33A85BA30632}">
   <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7:J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1852,12 +1943,24 @@
       <c r="B3" s="24">
         <v>0</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
+      <c r="C3" s="24">
+        <v>0</v>
+      </c>
+      <c r="D3" s="24">
+        <v>0</v>
+      </c>
+      <c r="E3" s="24">
+        <v>0</v>
+      </c>
+      <c r="F3" s="24">
+        <v>0</v>
+      </c>
+      <c r="G3" s="24">
+        <v>0</v>
+      </c>
+      <c r="H3" s="24">
+        <v>0</v>
+      </c>
       <c r="I3" s="24">
         <v>3</v>
       </c>
@@ -1885,6 +1988,24 @@
         <v>3</v>
       </c>
       <c r="B4" s="19">
+        <v>0</v>
+      </c>
+      <c r="C4" s="24">
+        <v>0</v>
+      </c>
+      <c r="D4" s="24">
+        <v>0</v>
+      </c>
+      <c r="E4" s="24">
+        <v>0</v>
+      </c>
+      <c r="F4" s="24">
+        <v>0</v>
+      </c>
+      <c r="G4" s="24">
+        <v>0</v>
+      </c>
+      <c r="H4" s="24">
         <v>0</v>
       </c>
       <c r="I4" s="24">
@@ -1916,6 +2037,45 @@
       <c r="B5" s="19">
         <v>0</v>
       </c>
+      <c r="C5" s="24">
+        <v>0</v>
+      </c>
+      <c r="D5" s="24">
+        <v>0</v>
+      </c>
+      <c r="E5" s="24">
+        <v>0</v>
+      </c>
+      <c r="F5" s="24">
+        <v>0</v>
+      </c>
+      <c r="G5" s="24">
+        <v>0</v>
+      </c>
+      <c r="H5" s="24">
+        <v>0</v>
+      </c>
+      <c r="I5" s="24">
+        <v>0</v>
+      </c>
+      <c r="J5" s="24">
+        <v>0</v>
+      </c>
+      <c r="K5" s="24">
+        <v>0</v>
+      </c>
+      <c r="L5" s="24">
+        <v>0</v>
+      </c>
+      <c r="M5" s="24">
+        <v>0</v>
+      </c>
+      <c r="N5" s="24">
+        <v>0</v>
+      </c>
+      <c r="O5" s="24">
+        <v>0</v>
+      </c>
       <c r="P5" s="19" t="s">
         <v>22</v>
       </c>
@@ -1927,8 +2087,24 @@
       <c r="B6" s="29">
         <v>0</v>
       </c>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
+      <c r="C6" s="24">
+        <v>0</v>
+      </c>
+      <c r="D6" s="24">
+        <v>0</v>
+      </c>
+      <c r="E6" s="24">
+        <v>0</v>
+      </c>
+      <c r="F6" s="24">
+        <v>0</v>
+      </c>
+      <c r="G6" s="24">
+        <v>0</v>
+      </c>
+      <c r="H6" s="24">
+        <v>0</v>
+      </c>
       <c r="I6" s="19">
         <f>I4/15</f>
         <v>166.66666666666666</v>
@@ -1937,10 +2113,21 @@
         <f>J4/15</f>
         <v>166.66666666666666</v>
       </c>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="29"/>
+      <c r="K6" s="24">
+        <v>0</v>
+      </c>
+      <c r="L6" s="24">
+        <v>0</v>
+      </c>
+      <c r="M6" s="24">
+        <v>0</v>
+      </c>
+      <c r="N6" s="24">
+        <v>0</v>
+      </c>
+      <c r="O6" s="24">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:18" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="27" t="s">
@@ -1949,14 +2136,30 @@
       <c r="B7" s="30">
         <v>0</v>
       </c>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
+      <c r="C7" s="24">
+        <v>0</v>
+      </c>
+      <c r="D7" s="24">
+        <v>0</v>
+      </c>
+      <c r="E7" s="24">
+        <v>0</v>
+      </c>
+      <c r="F7" s="24">
+        <v>0</v>
+      </c>
+      <c r="G7" s="24">
+        <v>0</v>
+      </c>
+      <c r="H7" s="24">
+        <v>0</v>
+      </c>
+      <c r="I7" s="24">
+        <v>0</v>
+      </c>
+      <c r="J7" s="24">
+        <v>0</v>
+      </c>
       <c r="K7" s="19">
         <f>K4/18</f>
         <v>138.88888888888889</v>
@@ -1985,12 +2188,24 @@
       <c r="B8" s="30">
         <v>0</v>
       </c>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
+      <c r="C8" s="24">
+        <v>0</v>
+      </c>
+      <c r="D8" s="24">
+        <v>0</v>
+      </c>
+      <c r="E8" s="24">
+        <v>0</v>
+      </c>
+      <c r="F8" s="24">
+        <v>0</v>
+      </c>
+      <c r="G8" s="24">
+        <v>0</v>
+      </c>
+      <c r="H8" s="24">
+        <v>0</v>
+      </c>
       <c r="I8" s="30">
         <v>15</v>
       </c>
@@ -2020,12 +2235,24 @@
       <c r="B9" s="31">
         <v>0</v>
       </c>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
+      <c r="C9" s="24">
+        <v>0</v>
+      </c>
+      <c r="D9" s="24">
+        <v>0</v>
+      </c>
+      <c r="E9" s="24">
+        <v>0</v>
+      </c>
+      <c r="F9" s="24">
+        <v>0</v>
+      </c>
+      <c r="G9" s="24">
+        <v>0</v>
+      </c>
+      <c r="H9" s="24">
+        <v>0</v>
+      </c>
       <c r="I9" s="30">
         <v>700</v>
       </c>
@@ -2058,12 +2285,24 @@
       <c r="B10" s="30">
         <v>0</v>
       </c>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
+      <c r="C10" s="24">
+        <v>0</v>
+      </c>
+      <c r="D10" s="24">
+        <v>0</v>
+      </c>
+      <c r="E10" s="24">
+        <v>0</v>
+      </c>
+      <c r="F10" s="24">
+        <v>0</v>
+      </c>
+      <c r="G10" s="24">
+        <v>0</v>
+      </c>
+      <c r="H10" s="24">
+        <v>0</v>
+      </c>
       <c r="I10" s="30">
         <f>SUM(I6:I7)</f>
         <v>166.66666666666666</v>
@@ -2100,12 +2339,24 @@
       <c r="B11" s="30">
         <v>0</v>
       </c>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30"/>
+      <c r="C11" s="24">
+        <v>0</v>
+      </c>
+      <c r="D11" s="24">
+        <v>0</v>
+      </c>
+      <c r="E11" s="24">
+        <v>0</v>
+      </c>
+      <c r="F11" s="24">
+        <v>0</v>
+      </c>
+      <c r="G11" s="24">
+        <v>0</v>
+      </c>
+      <c r="H11" s="24">
+        <v>0</v>
+      </c>
       <c r="I11" s="30">
         <f>I3</f>
         <v>3</v>
@@ -2142,12 +2393,24 @@
       <c r="B12" s="30">
         <v>0</v>
       </c>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
+      <c r="C12" s="24">
+        <v>0</v>
+      </c>
+      <c r="D12" s="24">
+        <v>0</v>
+      </c>
+      <c r="E12" s="24">
+        <v>0</v>
+      </c>
+      <c r="F12" s="24">
+        <v>0</v>
+      </c>
+      <c r="G12" s="24">
+        <v>0</v>
+      </c>
+      <c r="H12" s="24">
+        <v>0</v>
+      </c>
       <c r="I12" s="30">
         <f>I3</f>
         <v>3</v>
@@ -2184,12 +2447,24 @@
       <c r="B13" s="24">
         <v>0</v>
       </c>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
+      <c r="C13" s="24">
+        <v>0</v>
+      </c>
+      <c r="D13" s="24">
+        <v>0</v>
+      </c>
+      <c r="E13" s="24">
+        <v>0</v>
+      </c>
+      <c r="F13" s="24">
+        <v>0</v>
+      </c>
+      <c r="G13" s="24">
+        <v>0</v>
+      </c>
+      <c r="H13" s="24">
+        <v>0</v>
+      </c>
       <c r="I13" s="24">
         <v>600</v>
       </c>
@@ -2219,12 +2494,24 @@
       <c r="B14" s="24">
         <v>0</v>
       </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
+      <c r="C14" s="24">
+        <v>0</v>
+      </c>
+      <c r="D14" s="24">
+        <v>0</v>
+      </c>
+      <c r="E14" s="24">
+        <v>0</v>
+      </c>
+      <c r="F14" s="24">
+        <v>0</v>
+      </c>
+      <c r="G14" s="24">
+        <v>0</v>
+      </c>
+      <c r="H14" s="24">
+        <v>0</v>
+      </c>
       <c r="I14" s="24">
         <v>200</v>
       </c>
@@ -2254,12 +2541,24 @@
       <c r="B15" s="24">
         <v>0</v>
       </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
+      <c r="C15" s="24">
+        <v>0</v>
+      </c>
+      <c r="D15" s="24">
+        <v>0</v>
+      </c>
+      <c r="E15" s="24">
+        <v>0</v>
+      </c>
+      <c r="F15" s="24">
+        <v>0</v>
+      </c>
+      <c r="G15" s="24">
+        <v>0</v>
+      </c>
+      <c r="H15" s="24">
+        <v>0</v>
+      </c>
       <c r="I15" s="24">
         <f>I3</f>
         <v>3</v>
@@ -2296,12 +2595,24 @@
       <c r="B16" s="24">
         <v>0</v>
       </c>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
+      <c r="C16" s="24">
+        <v>0</v>
+      </c>
+      <c r="D16" s="24">
+        <v>0</v>
+      </c>
+      <c r="E16" s="24">
+        <v>0</v>
+      </c>
+      <c r="F16" s="24">
+        <v>0</v>
+      </c>
+      <c r="G16" s="24">
+        <v>0</v>
+      </c>
+      <c r="H16" s="24">
+        <v>0</v>
+      </c>
       <c r="I16" s="24">
         <f>I15*I14</f>
         <v>600</v>
@@ -2338,12 +2649,24 @@
       <c r="B17" s="24">
         <v>0</v>
       </c>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
+      <c r="C17" s="24">
+        <v>0</v>
+      </c>
+      <c r="D17" s="24">
+        <v>0</v>
+      </c>
+      <c r="E17" s="24">
+        <v>0</v>
+      </c>
+      <c r="F17" s="24">
+        <v>0</v>
+      </c>
+      <c r="G17" s="24">
+        <v>0</v>
+      </c>
+      <c r="H17" s="24">
+        <v>0</v>
+      </c>
       <c r="I17" s="24">
         <f>I3</f>
         <v>3</v>
@@ -2380,18 +2703,45 @@
       <c r="B18" s="24">
         <v>0</v>
       </c>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="24"/>
-      <c r="K18" s="24"/>
-      <c r="L18" s="24"/>
-      <c r="M18" s="24"/>
-      <c r="N18" s="24"/>
+      <c r="C18" s="24">
+        <v>0</v>
+      </c>
+      <c r="D18" s="24">
+        <v>0</v>
+      </c>
+      <c r="E18" s="24">
+        <v>0</v>
+      </c>
+      <c r="F18" s="24">
+        <v>0</v>
+      </c>
+      <c r="G18" s="24">
+        <v>0</v>
+      </c>
+      <c r="H18" s="24">
+        <v>0</v>
+      </c>
+      <c r="I18" s="24">
+        <v>0</v>
+      </c>
+      <c r="J18" s="24">
+        <v>0</v>
+      </c>
+      <c r="K18" s="24">
+        <v>0</v>
+      </c>
+      <c r="L18" s="24">
+        <v>0</v>
+      </c>
+      <c r="M18" s="24">
+        <v>0</v>
+      </c>
+      <c r="N18" s="24">
+        <v>0</v>
+      </c>
+      <c r="O18" s="24">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Formats and bugfix to 2 series bar cumulative comparison plots
</commit_message>
<xml_diff>
--- a/BAU_Floating_Gantt.xlsx
+++ b/BAU_Floating_Gantt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mshields\Documents\Projects\Supply Chain Roadmap\WETO requests\PTC_ITC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E290E850-F4C8-4F51-B12B-9AA39351A0C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F4C6443-4080-418C-8E38-5DCB5E26E3ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{53585B98-3EE9-4F0B-A243-A3207BC010B9}"/>
   </bookViews>
@@ -621,8 +621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99FEF727-7431-4502-9BF2-797477A5DFA8}">
   <dimension ref="A1:R22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22:O22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Final plots for PTC/ITC memo
</commit_message>
<xml_diff>
--- a/BAU_Floating_Gantt.xlsx
+++ b/BAU_Floating_Gantt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mshields\Documents\Projects\Supply Chain Roadmap\WETO requests\PTC_ITC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F4C6443-4080-418C-8E38-5DCB5E26E3ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0915FBE2-BB79-4D86-BEF7-48B5FC673501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{53585B98-3EE9-4F0B-A243-A3207BC010B9}"/>
+    <workbookView minimized="1" xWindow="2280" yWindow="2280" windowWidth="14400" windowHeight="7360" xr2:uid="{53585B98-3EE9-4F0B-A243-A3207BC010B9}"/>
   </bookViews>
   <sheets>
     <sheet name="BAU" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
   <si>
     <t>Project COD</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>substructure: Total OSP semisubs, #</t>
+  </si>
+  <si>
+    <t>Assume 2 km per turbine</t>
+  </si>
+  <si>
+    <t>Assume 50 km to shore and 2 cables per project</t>
   </si>
 </sst>
 </file>
@@ -621,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99FEF727-7431-4502-9BF2-797477A5DFA8}">
   <dimension ref="A1:R22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -781,44 +787,44 @@
       <c r="B4" s="1">
         <v>0</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="19">
         <v>1000</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="19">
         <v>2000</v>
       </c>
-      <c r="E4" s="1">
-        <v>2000</v>
-      </c>
-      <c r="F4" s="1">
-        <v>2000</v>
-      </c>
-      <c r="G4" s="1">
-        <v>2000</v>
-      </c>
-      <c r="H4" s="1">
-        <v>2000</v>
-      </c>
-      <c r="I4" s="1">
-        <v>2000</v>
-      </c>
-      <c r="J4" s="1">
-        <v>2000</v>
-      </c>
-      <c r="K4" s="1">
-        <v>2000</v>
-      </c>
-      <c r="L4" s="1">
-        <v>2000</v>
-      </c>
-      <c r="M4" s="1">
-        <v>2000</v>
-      </c>
-      <c r="N4" s="1">
-        <v>2000</v>
+      <c r="E4" s="19">
+        <v>2400</v>
+      </c>
+      <c r="F4" s="19">
+        <v>2400</v>
+      </c>
+      <c r="G4" s="19">
+        <v>2400</v>
+      </c>
+      <c r="H4" s="19">
+        <v>2400</v>
+      </c>
+      <c r="I4" s="19">
+        <v>2400</v>
+      </c>
+      <c r="J4" s="19">
+        <v>2400</v>
+      </c>
+      <c r="K4" s="19">
+        <v>2400</v>
+      </c>
+      <c r="L4" s="19">
+        <v>2400</v>
+      </c>
+      <c r="M4" s="19">
+        <v>2400</v>
+      </c>
+      <c r="N4" s="19">
+        <v>2400</v>
       </c>
       <c r="O4" s="19">
-        <v>2000</v>
+        <v>2400</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
@@ -833,7 +839,7 @@
         <v>83.333333333333329</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" ref="D5:E5" si="0">D4/12</f>
+        <f t="shared" ref="D5" si="0">D4/12</f>
         <v>166.66666666666666</v>
       </c>
       <c r="E5" s="24">
@@ -887,28 +893,28 @@
         <v>0</v>
       </c>
       <c r="E6" s="1">
-        <f>E4/15</f>
-        <v>133.33333333333334</v>
+        <f t="shared" ref="E6:J6" si="1">E4/15</f>
+        <v>160</v>
       </c>
       <c r="F6" s="1">
-        <f>F4/15</f>
-        <v>133.33333333333334</v>
+        <f t="shared" si="1"/>
+        <v>160</v>
       </c>
       <c r="G6" s="1">
-        <f>G4/15</f>
-        <v>133.33333333333334</v>
+        <f t="shared" si="1"/>
+        <v>160</v>
       </c>
       <c r="H6" s="1">
-        <f>H4/15</f>
-        <v>133.33333333333334</v>
+        <f t="shared" si="1"/>
+        <v>160</v>
       </c>
       <c r="I6" s="1">
-        <f>I4/15</f>
-        <v>133.33333333333334</v>
+        <f t="shared" si="1"/>
+        <v>160</v>
       </c>
       <c r="J6" s="1">
-        <f>J4/15</f>
-        <v>133.33333333333334</v>
+        <f t="shared" si="1"/>
+        <v>160</v>
       </c>
       <c r="K6" s="24">
         <v>0</v>
@@ -959,23 +965,23 @@
       </c>
       <c r="K7" s="1">
         <f>K4/18</f>
-        <v>111.11111111111111</v>
+        <v>133.33333333333334</v>
       </c>
       <c r="L7" s="1">
         <f>L4/18</f>
-        <v>111.11111111111111</v>
+        <v>133.33333333333334</v>
       </c>
       <c r="M7" s="1">
         <f>M4/18</f>
-        <v>111.11111111111111</v>
+        <v>133.33333333333334</v>
       </c>
       <c r="N7" s="1">
         <f>N4/18</f>
-        <v>111.11111111111111</v>
+        <v>133.33333333333334</v>
       </c>
       <c r="O7" s="19">
         <f>O4/18</f>
-        <v>111.11111111111111</v>
+        <v>133.33333333333334</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -1137,52 +1143,52 @@
         <v>62.5</v>
       </c>
       <c r="D11" s="30">
-        <f t="shared" ref="D11:O11" si="1">0.75*SUM(D$5:D$7)</f>
+        <f t="shared" ref="D11:O11" si="2">0.75*SUM(D$5:D$7)</f>
         <v>125</v>
       </c>
       <c r="E11" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
+        <v>120</v>
+      </c>
+      <c r="F11" s="30">
+        <f t="shared" si="2"/>
+        <v>120</v>
+      </c>
+      <c r="G11" s="30">
+        <f t="shared" si="2"/>
+        <v>120</v>
+      </c>
+      <c r="H11" s="30">
+        <f t="shared" si="2"/>
+        <v>120</v>
+      </c>
+      <c r="I11" s="30">
+        <f t="shared" si="2"/>
+        <v>120</v>
+      </c>
+      <c r="J11" s="30">
+        <f t="shared" si="2"/>
+        <v>120</v>
+      </c>
+      <c r="K11" s="30">
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
-      <c r="F11" s="30">
-        <f t="shared" si="1"/>
+      <c r="L11" s="30">
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
-      <c r="G11" s="30">
-        <f t="shared" si="1"/>
+      <c r="M11" s="30">
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
-      <c r="H11" s="30">
-        <f t="shared" si="1"/>
+      <c r="N11" s="30">
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
-      <c r="I11" s="30">
-        <f t="shared" si="1"/>
+      <c r="O11" s="30">
+        <f t="shared" si="2"/>
         <v>100</v>
-      </c>
-      <c r="J11" s="30">
-        <f t="shared" si="1"/>
-        <v>100</v>
-      </c>
-      <c r="K11" s="30">
-        <f t="shared" si="1"/>
-        <v>83.333333333333343</v>
-      </c>
-      <c r="L11" s="30">
-        <f t="shared" si="1"/>
-        <v>83.333333333333343</v>
-      </c>
-      <c r="M11" s="30">
-        <f t="shared" si="1"/>
-        <v>83.333333333333343</v>
-      </c>
-      <c r="N11" s="30">
-        <f t="shared" si="1"/>
-        <v>83.333333333333343</v>
-      </c>
-      <c r="O11" s="30">
-        <f t="shared" si="1"/>
-        <v>83.333333333333343</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -1197,52 +1203,52 @@
         <v>10.416666666666666</v>
       </c>
       <c r="D12" s="30">
-        <f t="shared" ref="D12:O13" si="2">0.125*SUM(D$5:D$7)</f>
+        <f t="shared" ref="D12:O13" si="3">0.125*SUM(D$5:D$7)</f>
         <v>20.833333333333332</v>
       </c>
       <c r="E12" s="30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="F12" s="30">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="G12" s="30">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="H12" s="30">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="I12" s="30">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="J12" s="30">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="K12" s="30">
+        <f t="shared" si="3"/>
         <v>16.666666666666668</v>
       </c>
-      <c r="F12" s="30">
-        <f t="shared" si="2"/>
+      <c r="L12" s="30">
+        <f t="shared" si="3"/>
         <v>16.666666666666668</v>
       </c>
-      <c r="G12" s="30">
-        <f t="shared" si="2"/>
+      <c r="M12" s="30">
+        <f t="shared" si="3"/>
         <v>16.666666666666668</v>
       </c>
-      <c r="H12" s="30">
-        <f t="shared" si="2"/>
+      <c r="N12" s="30">
+        <f t="shared" si="3"/>
         <v>16.666666666666668</v>
       </c>
-      <c r="I12" s="30">
-        <f t="shared" si="2"/>
+      <c r="O12" s="30">
+        <f t="shared" si="3"/>
         <v>16.666666666666668</v>
-      </c>
-      <c r="J12" s="30">
-        <f t="shared" si="2"/>
-        <v>16.666666666666668</v>
-      </c>
-      <c r="K12" s="30">
-        <f t="shared" si="2"/>
-        <v>13.888888888888889</v>
-      </c>
-      <c r="L12" s="30">
-        <f t="shared" si="2"/>
-        <v>13.888888888888889</v>
-      </c>
-      <c r="M12" s="30">
-        <f t="shared" si="2"/>
-        <v>13.888888888888889</v>
-      </c>
-      <c r="N12" s="30">
-        <f t="shared" si="2"/>
-        <v>13.888888888888889</v>
-      </c>
-      <c r="O12" s="30">
-        <f t="shared" si="2"/>
-        <v>13.888888888888889</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -1257,52 +1263,52 @@
         <v>10.416666666666666</v>
       </c>
       <c r="D13" s="30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>20.833333333333332</v>
       </c>
       <c r="E13" s="30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="F13" s="30">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="G13" s="30">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="H13" s="30">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="I13" s="30">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="J13" s="30">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="K13" s="30">
+        <f t="shared" si="3"/>
         <v>16.666666666666668</v>
       </c>
-      <c r="F13" s="30">
-        <f t="shared" si="2"/>
+      <c r="L13" s="30">
+        <f t="shared" si="3"/>
         <v>16.666666666666668</v>
       </c>
-      <c r="G13" s="30">
-        <f t="shared" si="2"/>
+      <c r="M13" s="30">
+        <f t="shared" si="3"/>
         <v>16.666666666666668</v>
       </c>
-      <c r="H13" s="30">
-        <f t="shared" si="2"/>
+      <c r="N13" s="30">
+        <f t="shared" si="3"/>
         <v>16.666666666666668</v>
       </c>
-      <c r="I13" s="30">
-        <f t="shared" si="2"/>
+      <c r="O13" s="30">
+        <f t="shared" si="3"/>
         <v>16.666666666666668</v>
-      </c>
-      <c r="J13" s="30">
-        <f t="shared" si="2"/>
-        <v>16.666666666666668</v>
-      </c>
-      <c r="K13" s="30">
-        <f t="shared" si="2"/>
-        <v>13.888888888888889</v>
-      </c>
-      <c r="L13" s="30">
-        <f t="shared" si="2"/>
-        <v>13.888888888888889</v>
-      </c>
-      <c r="M13" s="30">
-        <f t="shared" si="2"/>
-        <v>13.888888888888889</v>
-      </c>
-      <c r="N13" s="30">
-        <f t="shared" si="2"/>
-        <v>13.888888888888889</v>
-      </c>
-      <c r="O13" s="30">
-        <f t="shared" si="2"/>
-        <v>13.888888888888889</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -1317,51 +1323,51 @@
         <v>1</v>
       </c>
       <c r="D14" s="30">
-        <f t="shared" ref="D14:O14" si="3">D3</f>
+        <f t="shared" ref="D14:O14" si="4">D3</f>
         <v>3</v>
       </c>
       <c r="E14" s="30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="F14" s="30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="G14" s="30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="H14" s="30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="I14" s="30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="J14" s="30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="K14" s="30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="L14" s="30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="M14" s="30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="N14" s="30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="O14" s="30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
     </row>
@@ -1377,51 +1383,51 @@
         <v>1</v>
       </c>
       <c r="D15" s="30">
-        <f t="shared" ref="D15:O15" si="4">D3</f>
+        <f t="shared" ref="D15:O15" si="5">D3</f>
         <v>3</v>
       </c>
       <c r="E15" s="30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="F15" s="30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="G15" s="30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="H15" s="30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="I15" s="30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="J15" s="30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="K15" s="30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="L15" s="30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="M15" s="30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="N15" s="30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="O15" s="30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
     </row>
@@ -1484,51 +1490,51 @@
         <v>100</v>
       </c>
       <c r="D17" s="24">
-        <f t="shared" ref="D17:O17" si="5">100*D3</f>
+        <f t="shared" ref="D17:O17" si="6">100*D3</f>
         <v>300</v>
       </c>
       <c r="E17" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>300</v>
       </c>
       <c r="F17" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>300</v>
       </c>
       <c r="G17" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>300</v>
       </c>
       <c r="H17" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>300</v>
       </c>
       <c r="I17" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>300</v>
       </c>
       <c r="J17" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>300</v>
       </c>
       <c r="K17" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>300</v>
       </c>
       <c r="L17" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>300</v>
       </c>
       <c r="M17" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>300</v>
       </c>
       <c r="N17" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>300</v>
       </c>
       <c r="O17" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>300</v>
       </c>
     </row>
@@ -1544,51 +1550,51 @@
         <v>50</v>
       </c>
       <c r="D18" s="24">
-        <f t="shared" ref="D18:O18" si="6">50*D3</f>
+        <f t="shared" ref="D18:O18" si="7">50*D3</f>
         <v>150</v>
       </c>
       <c r="E18" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>150</v>
       </c>
       <c r="F18" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>150</v>
       </c>
       <c r="G18" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>150</v>
       </c>
       <c r="H18" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>150</v>
       </c>
       <c r="I18" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>150</v>
       </c>
       <c r="J18" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>150</v>
       </c>
       <c r="K18" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>150</v>
       </c>
       <c r="L18" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>150</v>
       </c>
       <c r="M18" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>150</v>
       </c>
       <c r="N18" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>150</v>
       </c>
       <c r="O18" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>150</v>
       </c>
     </row>
@@ -1600,56 +1606,56 @@
         <v>0</v>
       </c>
       <c r="C19" s="6">
-        <f>ROUNDUP(C4/350,0)</f>
-        <v>3</v>
+        <f>ROUNDUP(C4/500,0)</f>
+        <v>2</v>
       </c>
       <c r="D19" s="24">
-        <f t="shared" ref="D19:O19" si="7">ROUNDUP(D4/350,0)</f>
-        <v>6</v>
+        <f t="shared" ref="D19:O19" si="8">ROUNDUP(D4/500,0)</f>
+        <v>4</v>
       </c>
       <c r="E19" s="24">
-        <f t="shared" si="7"/>
-        <v>6</v>
+        <f t="shared" si="8"/>
+        <v>5</v>
       </c>
       <c r="F19" s="24">
-        <f t="shared" si="7"/>
-        <v>6</v>
+        <f t="shared" si="8"/>
+        <v>5</v>
       </c>
       <c r="G19" s="24">
-        <f t="shared" si="7"/>
-        <v>6</v>
+        <f t="shared" si="8"/>
+        <v>5</v>
       </c>
       <c r="H19" s="24">
-        <f t="shared" si="7"/>
-        <v>6</v>
+        <f t="shared" si="8"/>
+        <v>5</v>
       </c>
       <c r="I19" s="24">
-        <f t="shared" si="7"/>
-        <v>6</v>
+        <f t="shared" si="8"/>
+        <v>5</v>
       </c>
       <c r="J19" s="24">
-        <f t="shared" si="7"/>
-        <v>6</v>
+        <f t="shared" si="8"/>
+        <v>5</v>
       </c>
       <c r="K19" s="24">
-        <f t="shared" si="7"/>
-        <v>6</v>
+        <f t="shared" si="8"/>
+        <v>5</v>
       </c>
       <c r="L19" s="24">
-        <f t="shared" si="7"/>
-        <v>6</v>
+        <f t="shared" si="8"/>
+        <v>5</v>
       </c>
       <c r="M19" s="24">
-        <f t="shared" si="7"/>
-        <v>6</v>
+        <f t="shared" si="8"/>
+        <v>5</v>
       </c>
       <c r="N19" s="24">
-        <f t="shared" si="7"/>
-        <v>6</v>
+        <f t="shared" si="8"/>
+        <v>5</v>
       </c>
       <c r="O19" s="24">
-        <f t="shared" si="7"/>
-        <v>6</v>
+        <f t="shared" si="8"/>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -1661,55 +1667,55 @@
       </c>
       <c r="C20" s="6">
         <f>C18*C19</f>
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="D20" s="24">
-        <f t="shared" ref="D20:O20" si="8">D18*D19</f>
-        <v>900</v>
+        <f t="shared" ref="D20:O20" si="9">D18*D19</f>
+        <v>600</v>
       </c>
       <c r="E20" s="24">
-        <f t="shared" si="8"/>
-        <v>900</v>
+        <f t="shared" si="9"/>
+        <v>750</v>
       </c>
       <c r="F20" s="24">
-        <f t="shared" si="8"/>
-        <v>900</v>
+        <f t="shared" si="9"/>
+        <v>750</v>
       </c>
       <c r="G20" s="24">
-        <f t="shared" si="8"/>
-        <v>900</v>
+        <f t="shared" si="9"/>
+        <v>750</v>
       </c>
       <c r="H20" s="24">
-        <f t="shared" si="8"/>
-        <v>900</v>
+        <f t="shared" si="9"/>
+        <v>750</v>
       </c>
       <c r="I20" s="24">
-        <f t="shared" si="8"/>
-        <v>900</v>
+        <f t="shared" si="9"/>
+        <v>750</v>
       </c>
       <c r="J20" s="24">
-        <f t="shared" si="8"/>
-        <v>900</v>
+        <f t="shared" si="9"/>
+        <v>750</v>
       </c>
       <c r="K20" s="24">
-        <f t="shared" si="8"/>
-        <v>900</v>
+        <f t="shared" si="9"/>
+        <v>750</v>
       </c>
       <c r="L20" s="24">
-        <f t="shared" si="8"/>
-        <v>900</v>
+        <f t="shared" si="9"/>
+        <v>750</v>
       </c>
       <c r="M20" s="24">
-        <f t="shared" si="8"/>
-        <v>900</v>
+        <f t="shared" si="9"/>
+        <v>750</v>
       </c>
       <c r="N20" s="24">
-        <f t="shared" si="8"/>
-        <v>900</v>
+        <f t="shared" si="9"/>
+        <v>750</v>
       </c>
       <c r="O20" s="24">
-        <f t="shared" si="8"/>
-        <v>900</v>
+        <f t="shared" si="9"/>
+        <v>750</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -1724,51 +1730,51 @@
         <v>1</v>
       </c>
       <c r="D21" s="24">
-        <f t="shared" ref="D21:O21" si="9">D3</f>
+        <f t="shared" ref="D21:O21" si="10">D3</f>
         <v>3</v>
       </c>
       <c r="E21" s="24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="F21" s="24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="G21" s="24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="H21" s="24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="I21" s="24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="J21" s="24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="K21" s="24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="L21" s="24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="M21" s="24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="N21" s="24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="O21" s="24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
     </row>
@@ -1828,8 +1834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FBFDA7F-5F64-4EB0-B210-33A85BA30632}">
   <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7:J7"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2015,19 +2021,19 @@
         <v>2500</v>
       </c>
       <c r="K4" s="24">
-        <v>2500</v>
+        <v>1000</v>
       </c>
       <c r="L4" s="24">
-        <v>2500</v>
+        <v>0</v>
       </c>
       <c r="M4" s="24">
-        <v>2500</v>
+        <v>0</v>
       </c>
       <c r="N4" s="24">
-        <v>2500</v>
+        <v>0</v>
       </c>
       <c r="O4" s="24">
-        <v>2500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
@@ -2162,23 +2168,23 @@
       </c>
       <c r="K7" s="19">
         <f>K4/18</f>
-        <v>138.88888888888889</v>
+        <v>55.555555555555557</v>
       </c>
       <c r="L7" s="19">
         <f t="shared" ref="L7:O7" si="0">L4/18</f>
-        <v>138.88888888888889</v>
+        <v>0</v>
       </c>
       <c r="M7" s="19">
         <f t="shared" si="0"/>
-        <v>138.88888888888889</v>
+        <v>0</v>
       </c>
       <c r="N7" s="19">
         <f t="shared" si="0"/>
-        <v>138.88888888888889</v>
+        <v>0</v>
       </c>
       <c r="O7" s="19">
         <f t="shared" si="0"/>
-        <v>138.88888888888889</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2313,23 +2319,23 @@
       </c>
       <c r="K10" s="30">
         <f t="shared" si="1"/>
-        <v>138.88888888888889</v>
+        <v>55.555555555555557</v>
       </c>
       <c r="L10" s="30">
         <f t="shared" si="1"/>
-        <v>138.88888888888889</v>
+        <v>0</v>
       </c>
       <c r="M10" s="30">
         <f t="shared" si="1"/>
-        <v>138.88888888888889</v>
+        <v>0</v>
       </c>
       <c r="N10" s="30">
         <f t="shared" si="1"/>
-        <v>138.88888888888889</v>
+        <v>0</v>
       </c>
       <c r="O10" s="30">
         <f t="shared" si="1"/>
-        <v>138.88888888888889</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2466,25 +2472,35 @@
         <v>0</v>
       </c>
       <c r="I13" s="24">
-        <v>600</v>
+        <f>2*I6</f>
+        <v>333.33333333333331</v>
       </c>
       <c r="J13" s="24">
-        <v>600</v>
+        <f>2*J6</f>
+        <v>333.33333333333331</v>
       </c>
       <c r="K13" s="24">
-        <v>600</v>
+        <f>2*K7</f>
+        <v>111.11111111111111</v>
       </c>
       <c r="L13" s="24">
-        <v>600</v>
+        <f t="shared" ref="L13:O13" si="4">2*L7</f>
+        <v>0</v>
       </c>
       <c r="M13" s="24">
-        <v>600</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="N13" s="24">
-        <v>600</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="O13" s="24">
-        <v>600</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P13" s="19" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2533,6 +2549,9 @@
       <c r="O14" s="24">
         <v>200</v>
       </c>
+      <c r="P14" s="19" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="15" spans="1:18" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="20" t="s">
@@ -2560,32 +2579,25 @@
         <v>0</v>
       </c>
       <c r="I15" s="24">
-        <f>I3</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J15" s="24">
-        <f t="shared" ref="J15:O15" si="4">J3</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K15" s="24">
-        <f t="shared" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L15" s="24">
-        <f t="shared" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M15" s="24">
-        <f t="shared" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N15" s="24">
-        <f t="shared" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O15" s="24">
-        <f t="shared" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2615,31 +2627,31 @@
       </c>
       <c r="I16" s="24">
         <f>I15*I14</f>
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="J16" s="24">
         <f t="shared" ref="J16:O16" si="5">J15*J14</f>
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="K16" s="24">
         <f t="shared" si="5"/>
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="L16" s="24">
         <f t="shared" si="5"/>
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="M16" s="24">
         <f t="shared" si="5"/>
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="N16" s="24">
         <f t="shared" si="5"/>
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="O16" s="24">
         <f t="shared" si="5"/>
-        <v>600</v>
+        <v>400</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -2668,32 +2680,25 @@
         <v>0</v>
       </c>
       <c r="I17" s="24">
-        <f>I3</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J17" s="24">
-        <f t="shared" ref="J17:O17" si="6">J3</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K17" s="24">
-        <f t="shared" si="6"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L17" s="24">
-        <f t="shared" si="6"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M17" s="24">
-        <f t="shared" si="6"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N17" s="24">
-        <f t="shared" si="6"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O17" s="24">
-        <f t="shared" si="6"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.35">

</xml_diff>